<commit_message>
New Microsoft Excel Worksheet.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/New Microsoft Excel Worksheet.xlsx
+++ b/Documentation/New Microsoft Excel Worksheet.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -114,7 +114,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +149,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -333,7 +333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>